<commit_message>
addin class data analysis with penalty analysis in it
</commit_message>
<xml_diff>
--- a/tests/VN8413_Data_Rawdata.xlsx
+++ b/tests/VN8413_Data_Rawdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/723e82af93afbbb8/Dev Area/PyPackages/packaging_dpkits/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_C929E6B904BA0AC8A075C72F089BC069A612D362" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{550BB14C-1CE8-4975-8C59-9ABF708136FD}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_C929E6B904BA0AC8A075C72F089BC069A612D362" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0872499B-0A3D-4F0C-9E6B-08CC33674F58}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stack_Rawdata" sheetId="1" r:id="rId1"/>
@@ -4386,12 +4386,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -4421,7 +4427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4432,6 +4438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4447,6 +4454,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4736,7 +4747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -42494,9 +42505,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="95.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -42750,17 +42767,17 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>1247</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="4" t="s">
         <v>1271</v>
       </c>
     </row>
@@ -42792,59 +42809,59 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>1274</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>1247</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="4" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>1276</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>1247</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="4" t="s">
         <v>1277</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>1278</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>1247</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
         <v>1279</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>1280</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>1247</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="4" t="s">
         <v>1281</v>
       </c>
     </row>
@@ -42876,17 +42893,17 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>1284</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="4" t="s">
         <v>1247</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="4" t="s">
         <v>1281</v>
       </c>
     </row>

</xml_diff>